<commit_message>
ajuste na figura echo
</commit_message>
<xml_diff>
--- a/echo_scores.xlsx
+++ b/echo_scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e4b858b1fb629067/Documentos/Quality_of_life_in_MISC_pediatric/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{BDE90983-EA8B-45F7-9753-AC9C6535C778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E73442D-FB8D-4A62-B87B-FF7720EBE599}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="8_{BDE90983-EA8B-45F7-9753-AC9C6535C778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC329999-8C60-4805-8477-B6549BADF2C5}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B4645AE-5123-9940-9F82-F0920807FCE0}"/>
+    <workbookView xWindow="-108" yWindow="864" windowWidth="17280" windowHeight="8880" xr2:uid="{1B4645AE-5123-9940-9F82-F0920807FCE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="118">
   <si>
     <t>id</t>
   </si>
@@ -357,6 +357,39 @@
   </si>
   <si>
     <t>-1.50</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>0.49</t>
+  </si>
+  <si>
+    <t>2.62</t>
+  </si>
+  <si>
+    <t>LV_mass_z score</t>
+  </si>
+  <si>
+    <t>-1.05</t>
+  </si>
+  <si>
+    <t>-1.36</t>
+  </si>
+  <si>
+    <t>1.48</t>
+  </si>
+  <si>
+    <t>0.33</t>
+  </si>
+  <si>
+    <t>1.53</t>
+  </si>
+  <si>
+    <t>1.76</t>
+  </si>
+  <si>
+    <t>0.68</t>
   </si>
 </sst>
 </file>
@@ -418,9 +451,11 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92510E36-63DD-3549-80D9-F97E5E7F171D}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,6 +821,9 @@
       <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="M1" s="7" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -824,7 +862,9 @@
       <c r="L2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M2" s="5"/>
+      <c r="M2" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -860,10 +900,12 @@
       <c r="K3" s="5">
         <v>78</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="M3" s="5"/>
+      <c r="M3" s="6" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -887,7 +929,7 @@
       <c r="G4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>106</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -902,7 +944,9 @@
       <c r="L4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="6" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -941,7 +985,9 @@
       <c r="L5" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="M5" s="6"/>
+      <c r="M5" s="5" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -980,7 +1026,9 @@
       <c r="L6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="M6" s="6"/>
+      <c r="M6" s="5" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1016,10 +1064,12 @@
       <c r="K7" s="5">
         <v>79</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="M7" s="5"/>
+      <c r="M7" s="5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1043,7 +1093,7 @@
       <c r="G8" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>104</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -1055,10 +1105,12 @@
       <c r="K8" s="5">
         <v>62</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="M8" s="5"/>
+      <c r="M8" s="5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1094,10 +1146,12 @@
       <c r="K9" s="5">
         <v>73</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="L9" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="M9" s="5"/>
+      <c r="M9" s="5" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1121,7 +1175,7 @@
       <c r="G10" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>105</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -1133,10 +1187,12 @@
       <c r="K10" s="5">
         <v>63</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="M10" s="5"/>
+      <c r="M10" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1172,10 +1228,12 @@
       <c r="K11" s="5">
         <v>65</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="M11" s="5"/>
+      <c r="M11" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1211,10 +1269,12 @@
       <c r="K12" s="5">
         <v>70</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="L12" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="M12" s="5"/>
+      <c r="M12" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1253,7 +1313,9 @@
       <c r="L13" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="M13" s="6"/>
+      <c r="M13" s="5" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>